<commit_message>
add VE tables to XLS and WIP of the E85 Cranking fuel entrichment
</commit_message>
<xml_diff>
--- a/AFR-Tables/MazdaEdit-AFR-231HP.xlsx
+++ b/AFR-Tables/MazdaEdit-AFR-231HP.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\AFR-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{105E6211-5D65-4623-8284-84E603610709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3591F6B5-DC2E-43F7-893E-983DCF56B687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{37191EE4-084A-455C-847F-C07633C08EC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{37191EE4-084A-455C-847F-C07633C08EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="AFR 1 (RX8 Evolve 2006 UK)" sheetId="2" r:id="rId1"/>
     <sheet name="AFR 2 (RX8 Evolve 2006 UK)" sheetId="3" r:id="rId2"/>
     <sheet name="AFR 3 (RX8 Evolve 2006 UK)" sheetId="4" r:id="rId3"/>
+    <sheet name="Volumetry Efficienccy " sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3406,7 +3407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B7775-635C-4DB8-935C-614356DD0AF8}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -4773,4 +4774,1139 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D095E2F3-83EB-429F-AAB5-321D962BD99C}">
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1.0792999999999999</v>
+      </c>
+      <c r="B1">
+        <v>1.0792999999999999</v>
+      </c>
+      <c r="C1">
+        <v>1.0556000000000001</v>
+      </c>
+      <c r="D1">
+        <v>1.0704</v>
+      </c>
+      <c r="E1">
+        <v>1.0382</v>
+      </c>
+      <c r="F1">
+        <v>1.0286</v>
+      </c>
+      <c r="G1">
+        <v>1.0496000000000001</v>
+      </c>
+      <c r="H1">
+        <v>1.0505</v>
+      </c>
+      <c r="I1">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="J1">
+        <v>0.97360000000000002</v>
+      </c>
+      <c r="K1">
+        <v>0.96150000000000002</v>
+      </c>
+      <c r="L1">
+        <v>1.0179</v>
+      </c>
+      <c r="M1">
+        <v>1.1039000000000001</v>
+      </c>
+      <c r="N1">
+        <v>0.99329999999999996</v>
+      </c>
+      <c r="O1">
+        <v>0.99870000000000003</v>
+      </c>
+      <c r="P1">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="Q1">
+        <v>1.0017</v>
+      </c>
+      <c r="R1">
+        <v>1.0154000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.0792999999999999</v>
+      </c>
+      <c r="B2">
+        <v>1.0792999999999999</v>
+      </c>
+      <c r="C2">
+        <v>1.0596000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.0205</v>
+      </c>
+      <c r="E2">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="F2">
+        <v>1.0293000000000001</v>
+      </c>
+      <c r="G2">
+        <v>1.0368999999999999</v>
+      </c>
+      <c r="H2">
+        <v>1.022</v>
+      </c>
+      <c r="I2">
+        <v>0.96430000000000005</v>
+      </c>
+      <c r="J2">
+        <v>0.97130000000000005</v>
+      </c>
+      <c r="K2">
+        <v>0.96409999999999996</v>
+      </c>
+      <c r="L2">
+        <v>1.0316000000000001</v>
+      </c>
+      <c r="M2">
+        <v>1.1039000000000001</v>
+      </c>
+      <c r="N2">
+        <v>0.99329999999999996</v>
+      </c>
+      <c r="O2">
+        <v>0.99870000000000003</v>
+      </c>
+      <c r="P2">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="Q2">
+        <v>1.0017</v>
+      </c>
+      <c r="R2">
+        <v>1.0154000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.0616000000000001</v>
+      </c>
+      <c r="B3">
+        <v>1.0616000000000001</v>
+      </c>
+      <c r="C3">
+        <v>1.0556000000000001</v>
+      </c>
+      <c r="D3">
+        <v>1.0125999999999999</v>
+      </c>
+      <c r="E3">
+        <v>1.0095000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.0165</v>
+      </c>
+      <c r="G3">
+        <v>1.0367999999999999</v>
+      </c>
+      <c r="H3">
+        <v>1.0135000000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.96679999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.96909999999999996</v>
+      </c>
+      <c r="K3">
+        <v>0.9667</v>
+      </c>
+      <c r="L3">
+        <v>1.0452999999999999</v>
+      </c>
+      <c r="M3">
+        <v>1.0504</v>
+      </c>
+      <c r="N3">
+        <v>0.99329999999999996</v>
+      </c>
+      <c r="O3">
+        <v>0.99870000000000003</v>
+      </c>
+      <c r="P3">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="Q3">
+        <v>1.0017</v>
+      </c>
+      <c r="R3">
+        <v>1.0154000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.0609</v>
+      </c>
+      <c r="B4">
+        <v>1.0609</v>
+      </c>
+      <c r="C4">
+        <v>1.0295000000000001</v>
+      </c>
+      <c r="D4">
+        <v>1.0024</v>
+      </c>
+      <c r="E4">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="F4">
+        <v>1.0135000000000001</v>
+      </c>
+      <c r="G4">
+        <v>1.0116000000000001</v>
+      </c>
+      <c r="H4">
+        <v>0.99650000000000005</v>
+      </c>
+      <c r="I4">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="J4">
+        <v>0.9556</v>
+      </c>
+      <c r="K4">
+        <v>0.96230000000000004</v>
+      </c>
+      <c r="L4">
+        <v>1.0219</v>
+      </c>
+      <c r="M4">
+        <v>0.997</v>
+      </c>
+      <c r="N4">
+        <v>1.0277000000000001</v>
+      </c>
+      <c r="O4">
+        <v>1.0075000000000001</v>
+      </c>
+      <c r="P4">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="Q4">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="R4">
+        <v>0.99580000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.0555000000000001</v>
+      </c>
+      <c r="B5">
+        <v>1.0555000000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.0176000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="E5">
+        <v>0.97760000000000002</v>
+      </c>
+      <c r="F5">
+        <v>1.004</v>
+      </c>
+      <c r="G5">
+        <v>0.98050000000000004</v>
+      </c>
+      <c r="H5">
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="I5">
+        <v>0.97250000000000003</v>
+      </c>
+      <c r="J5">
+        <v>0.94210000000000005</v>
+      </c>
+      <c r="K5">
+        <v>0.9698</v>
+      </c>
+      <c r="L5">
+        <v>0.9839</v>
+      </c>
+      <c r="M5">
+        <v>1.0055000000000001</v>
+      </c>
+      <c r="N5">
+        <v>1.0474000000000001</v>
+      </c>
+      <c r="O5">
+        <v>1.0105</v>
+      </c>
+      <c r="P5">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="Q5">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="R5">
+        <v>0.98099999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.0532999999999999</v>
+      </c>
+      <c r="B6">
+        <v>1.0532999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.99729999999999996</v>
+      </c>
+      <c r="D6">
+        <v>0.97460000000000002</v>
+      </c>
+      <c r="E6">
+        <v>0.96989999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.98450000000000004</v>
+      </c>
+      <c r="G6">
+        <v>0.96540000000000004</v>
+      </c>
+      <c r="H6">
+        <v>0.96260000000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.96860000000000002</v>
+      </c>
+      <c r="J6">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="K6">
+        <v>0.94650000000000001</v>
+      </c>
+      <c r="L6">
+        <v>1.0122</v>
+      </c>
+      <c r="M6">
+        <v>1.0246</v>
+      </c>
+      <c r="N6">
+        <v>1.0498000000000001</v>
+      </c>
+      <c r="O6">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="P6">
+        <v>0.9879</v>
+      </c>
+      <c r="Q6">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="R6">
+        <v>1.0203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.0528</v>
+      </c>
+      <c r="B7">
+        <v>1.0528</v>
+      </c>
+      <c r="C7">
+        <v>0.99270000000000003</v>
+      </c>
+      <c r="D7">
+        <v>0.96750000000000003</v>
+      </c>
+      <c r="E7">
+        <v>0.9677</v>
+      </c>
+      <c r="F7">
+        <v>0.9708</v>
+      </c>
+      <c r="G7">
+        <v>0.9617</v>
+      </c>
+      <c r="H7">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="I7">
+        <v>0.95530000000000004</v>
+      </c>
+      <c r="J7">
+        <v>0.94710000000000005</v>
+      </c>
+      <c r="K7">
+        <v>0.93289999999999995</v>
+      </c>
+      <c r="L7">
+        <v>1.0148999999999999</v>
+      </c>
+      <c r="M7">
+        <v>1.0106999999999999</v>
+      </c>
+      <c r="N7">
+        <v>1.0251999999999999</v>
+      </c>
+      <c r="O7">
+        <v>0.98</v>
+      </c>
+      <c r="P7">
+        <v>1.0056</v>
+      </c>
+      <c r="Q7">
+        <v>0.9889</v>
+      </c>
+      <c r="R7">
+        <v>1.0056</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.0291999999999999</v>
+      </c>
+      <c r="B8">
+        <v>1.0291999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.97850000000000004</v>
+      </c>
+      <c r="D8">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="E8">
+        <v>0.97089999999999999</v>
+      </c>
+      <c r="F8">
+        <v>0.96179999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="H8">
+        <v>0.95209999999999995</v>
+      </c>
+      <c r="I8">
+        <v>0.94369999999999998</v>
+      </c>
+      <c r="J8">
+        <v>0.9325</v>
+      </c>
+      <c r="K8">
+        <v>0.97709999999999997</v>
+      </c>
+      <c r="L8">
+        <v>1.0119</v>
+      </c>
+      <c r="M8">
+        <v>1.0007999999999999</v>
+      </c>
+      <c r="N8">
+        <v>0.99329999999999996</v>
+      </c>
+      <c r="O8">
+        <v>1.0056</v>
+      </c>
+      <c r="P8">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="Q8">
+        <v>0.9859</v>
+      </c>
+      <c r="R8">
+        <v>0.99580000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.0056</v>
+      </c>
+      <c r="B9">
+        <v>1.0056</v>
+      </c>
+      <c r="C9">
+        <v>0.96430000000000005</v>
+      </c>
+      <c r="D9">
+        <v>0.95779999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.97970000000000002</v>
+      </c>
+      <c r="F9">
+        <v>0.96179999999999999</v>
+      </c>
+      <c r="G9">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="H9">
+        <v>0.94869999999999999</v>
+      </c>
+      <c r="I9">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="J9">
+        <v>0.97689999999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="L9">
+        <v>1.0002</v>
+      </c>
+      <c r="M9">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="N9">
+        <v>1.0326</v>
+      </c>
+      <c r="O9">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="P9">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="Q9">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="R9">
+        <v>0.97609999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="B10">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="C10">
+        <v>0.96909999999999996</v>
+      </c>
+      <c r="D10">
+        <v>0.94330000000000003</v>
+      </c>
+      <c r="E10">
+        <v>0.96309999999999996</v>
+      </c>
+      <c r="F10">
+        <v>0.94269999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.95309999999999995</v>
+      </c>
+      <c r="H10">
+        <v>0.94450000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.95109999999999995</v>
+      </c>
+      <c r="J10">
+        <v>0.9597</v>
+      </c>
+      <c r="K10">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="L10">
+        <v>0.98839999999999995</v>
+      </c>
+      <c r="M10">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="N10">
+        <v>1.0179</v>
+      </c>
+      <c r="O10">
+        <v>0.9879</v>
+      </c>
+      <c r="P10">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="Q10">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="R10">
+        <v>0.96630000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.9859</v>
+      </c>
+      <c r="B11">
+        <v>0.9859</v>
+      </c>
+      <c r="C11">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.94269999999999998</v>
+      </c>
+      <c r="E11">
+        <v>0.9466</v>
+      </c>
+      <c r="F11">
+        <v>0.92359999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.93240000000000001</v>
+      </c>
+      <c r="H11">
+        <v>0.93610000000000004</v>
+      </c>
+      <c r="I11">
+        <v>0.95209999999999995</v>
+      </c>
+      <c r="J11">
+        <v>0.97030000000000005</v>
+      </c>
+      <c r="K11">
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="L11">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="M11">
+        <v>0.99329999999999996</v>
+      </c>
+      <c r="N11">
+        <v>0.99329999999999996</v>
+      </c>
+      <c r="O11">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="P11">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="R11">
+        <v>0.96630000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.9859</v>
+      </c>
+      <c r="B12">
+        <v>0.9859</v>
+      </c>
+      <c r="C12">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E12">
+        <v>0.9073</v>
+      </c>
+      <c r="F12">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="G12">
+        <v>0.9133</v>
+      </c>
+      <c r="H12">
+        <v>0.92579999999999996</v>
+      </c>
+      <c r="I12">
+        <v>0.93510000000000004</v>
+      </c>
+      <c r="J12">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.98350000000000004</v>
+      </c>
+      <c r="L12">
+        <v>0.9859</v>
+      </c>
+      <c r="M12">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="N12">
+        <v>0.97860000000000003</v>
+      </c>
+      <c r="O12">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="P12">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="Q12">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="R12">
+        <v>0.9466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.9859</v>
+      </c>
+      <c r="B13">
+        <v>0.9859</v>
+      </c>
+      <c r="C13">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E13">
+        <v>0.9073</v>
+      </c>
+      <c r="F13">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G13">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="H13">
+        <v>0.91020000000000001</v>
+      </c>
+      <c r="I13">
+        <v>0.92920000000000003</v>
+      </c>
+      <c r="J13">
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="K13">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="L13">
+        <v>0.97860000000000003</v>
+      </c>
+      <c r="M13">
+        <v>0.96870000000000001</v>
+      </c>
+      <c r="N13">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="O13">
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="P13">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="Q13">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="R13">
+        <v>0.95840000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.9859</v>
+      </c>
+      <c r="B14">
+        <v>0.9859</v>
+      </c>
+      <c r="C14">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D14">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E14">
+        <v>0.9073</v>
+      </c>
+      <c r="F14">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G14">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H14">
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="I14">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="J14">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="K14">
+        <v>0.97119999999999995</v>
+      </c>
+      <c r="L14">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="M14">
+        <v>0.94910000000000005</v>
+      </c>
+      <c r="N14">
+        <v>0.96870000000000001</v>
+      </c>
+      <c r="O14">
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="P14">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="Q14">
+        <v>0.97319999999999995</v>
+      </c>
+      <c r="R14">
+        <v>0.97609999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.9859</v>
+      </c>
+      <c r="B15">
+        <v>0.9859</v>
+      </c>
+      <c r="C15">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D15">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E15">
+        <v>0.9073</v>
+      </c>
+      <c r="F15">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G15">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H15">
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="I15">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="J15">
+        <v>0.96060000000000001</v>
+      </c>
+      <c r="K15">
+        <v>0.97119999999999995</v>
+      </c>
+      <c r="L15">
+        <v>0.9627</v>
+      </c>
+      <c r="M15">
+        <v>0.94189999999999996</v>
+      </c>
+      <c r="N15">
+        <v>0.96509999999999996</v>
+      </c>
+      <c r="O15">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="P15">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="Q15">
+        <v>0.97319999999999995</v>
+      </c>
+      <c r="R15">
+        <v>0.89390000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.9859</v>
+      </c>
+      <c r="B16">
+        <v>0.9859</v>
+      </c>
+      <c r="C16">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E16">
+        <v>0.9073</v>
+      </c>
+      <c r="F16">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G16">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H16">
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="I16">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="J16">
+        <v>0.95960000000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.94740000000000002</v>
+      </c>
+      <c r="L16">
+        <v>0.96140000000000003</v>
+      </c>
+      <c r="M16">
+        <v>0.93920000000000003</v>
+      </c>
+      <c r="N16">
+        <v>0.95450000000000002</v>
+      </c>
+      <c r="O16">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="P16">
+        <v>0.96479999999999999</v>
+      </c>
+      <c r="Q16">
+        <v>0.93510000000000004</v>
+      </c>
+      <c r="R16">
+        <v>0.89190000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.9859</v>
+      </c>
+      <c r="B17">
+        <v>0.9859</v>
+      </c>
+      <c r="C17">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D17">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E17">
+        <v>0.9073</v>
+      </c>
+      <c r="F17">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H17">
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="I17">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="J17">
+        <v>0.95850000000000002</v>
+      </c>
+      <c r="K17">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="L17">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="M17">
+        <v>0.92479999999999996</v>
+      </c>
+      <c r="N17">
+        <v>0.94320000000000004</v>
+      </c>
+      <c r="O17">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="P17">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="Q17">
+        <v>0.89449999999999996</v>
+      </c>
+      <c r="R17">
+        <v>0.88970000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.9859</v>
+      </c>
+      <c r="B18">
+        <v>0.9859</v>
+      </c>
+      <c r="C18">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E18">
+        <v>0.9073</v>
+      </c>
+      <c r="F18">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G18">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H18">
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="I18">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="J18">
+        <v>0.95589999999999997</v>
+      </c>
+      <c r="K18">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="L18">
+        <v>0.91259999999999997</v>
+      </c>
+      <c r="M18">
+        <v>0.89049999999999996</v>
+      </c>
+      <c r="N18">
+        <v>0.91610000000000003</v>
+      </c>
+      <c r="O18">
+        <v>0.92989999999999995</v>
+      </c>
+      <c r="P18">
+        <v>0.9254</v>
+      </c>
+      <c r="Q18">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="R18">
+        <v>0.88460000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.9859</v>
+      </c>
+      <c r="B19">
+        <v>0.9859</v>
+      </c>
+      <c r="C19">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D19">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E19">
+        <v>0.9073</v>
+      </c>
+      <c r="F19">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H19">
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="I19">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="J19">
+        <v>0.95069999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="L19">
+        <v>0.90080000000000005</v>
+      </c>
+      <c r="M19">
+        <v>0.87870000000000004</v>
+      </c>
+      <c r="N19">
+        <v>0.90429999999999999</v>
+      </c>
+      <c r="O19">
+        <v>0.91810000000000003</v>
+      </c>
+      <c r="P19">
+        <v>0.91220000000000001</v>
+      </c>
+      <c r="Q19">
+        <v>0.87490000000000001</v>
+      </c>
+      <c r="R19">
+        <v>0.87419999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.9859</v>
+      </c>
+      <c r="B20">
+        <v>0.9859</v>
+      </c>
+      <c r="C20">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E20">
+        <v>0.9073</v>
+      </c>
+      <c r="F20">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H20">
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="I20">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="J20">
+        <v>0.95069999999999999</v>
+      </c>
+      <c r="K20">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="L20">
+        <v>0.89290000000000003</v>
+      </c>
+      <c r="M20">
+        <v>0.87080000000000002</v>
+      </c>
+      <c r="N20">
+        <v>0.89649999999999996</v>
+      </c>
+      <c r="O20">
+        <v>0.91020000000000001</v>
+      </c>
+      <c r="P20">
+        <v>0.91220000000000001</v>
+      </c>
+      <c r="Q20">
+        <v>0.87490000000000001</v>
+      </c>
+      <c r="R20">
+        <v>0.87419999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>